<commit_message>
Removed visitors from the future section
</commit_message>
<xml_diff>
--- a/Copenhagen/Copenhagen_2022/data/Copenhagen_clean.xlsx
+++ b/Copenhagen/Copenhagen_2022/data/Copenhagen_clean.xlsx
@@ -16016,7 +16016,9 @@
       <c r="AN122" s="1" t="n">
         <v>39032</v>
       </c>
-      <c r="AO122" s="1"/>
+      <c r="AO122" s="1" t="n">
+        <v>39032</v>
+      </c>
       <c r="AP122" s="1" t="n">
         <v>39032.75</v>
       </c>
@@ -28764,7 +28766,9 @@
       <c r="AN222" s="1" t="n">
         <v>39032</v>
       </c>
-      <c r="AO222" s="1"/>
+      <c r="AO222" s="1" t="n">
+        <v>39032</v>
+      </c>
       <c r="AP222" s="1" t="n">
         <v>39032.75</v>
       </c>

</xml_diff>